<commit_message>
Update project part 2
</commit_message>
<xml_diff>
--- a/data/newfoundland_fishing_labour_force.xlsx
+++ b/data/newfoundland_fishing_labour_force.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelly\Documents\grad\Telling Stories with Data\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3372FD96-BD98-4E5D-94B3-0169DAE5B0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110D7280-0E9B-447F-8708-C9B5200931C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{09B1A3CD-C43F-4BB1-ACB7-80607F7E19BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Percent Fisherman</t>
+  </si>
+  <si>
+    <t>Non-Fishers</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67C9E7D-A004-4A44-8963-BB455F54EA39}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1355,7 +1358,7 @@
     <col min="3" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1368,8 +1371,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1857</v>
       </c>
@@ -1382,8 +1388,12 @@
       <c r="D2">
         <v>90.4</v>
       </c>
+      <c r="E2">
+        <f>C2-B2</f>
+        <v>4093</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1901</v>
       </c>
@@ -1396,8 +1406,12 @@
       <c r="D3">
         <v>61.2</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">C3-B3</f>
+        <v>26137</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1945</v>
       </c>
@@ -1410,8 +1424,12 @@
       <c r="D4">
         <v>31</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>70265</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1951</v>
       </c>
@@ -1424,8 +1442,12 @@
       <c r="D5">
         <v>17.2</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>88069</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1961</v>
       </c>
@@ -1438,8 +1460,12 @@
       <c r="D6">
         <v>7.3</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>104127</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1971</v>
       </c>
@@ -1452,8 +1478,12 @@
       <c r="D7">
         <v>4.9000000000000004</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>140730</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1981</v>
       </c>
@@ -1466,8 +1496,12 @@
       <c r="D8">
         <v>5.4</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>210445</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1991</v>
       </c>
@@ -1480,8 +1514,12 @@
       <c r="D9">
         <v>4.8</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>254465</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2001</v>
       </c>
@@ -1493,6 +1531,10 @@
       </c>
       <c r="D10">
         <v>4.5999999999999996</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>230425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>